<commit_message>
Add tests case for cars_owners
</commit_message>
<xml_diff>
--- a/tests/car_owners_files/car_owners_valid.xlsx
+++ b/tests/car_owners_files/car_owners_valid.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Олеся\Desktop\Цифровой прорыв\lonely-eye\tests\car_owners_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90A3D776-706E-49D7-9D80-2AB62892F8A6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE2A0144-3643-403F-AD8F-05D1EA38A4C8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t>У254УА797</t>
   </si>
@@ -94,6 +94,12 @@
   </si>
   <si>
     <t>number</t>
+  </si>
+  <si>
+    <t>awdawd@test.com</t>
+  </si>
+  <si>
+    <t>dawdaw@tesd.tv</t>
   </si>
 </sst>
 </file>
@@ -424,7 +430,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -485,6 +493,9 @@
       <c r="B4" s="1" t="s">
         <v>11</v>
       </c>
+      <c r="C4">
+        <v>89036054939</v>
+      </c>
       <c r="D4" s="1" t="s">
         <v>14</v>
       </c>
@@ -496,7 +507,9 @@
       <c r="A5" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="1"/>
+      <c r="B5" s="1" t="s">
+        <v>23</v>
+      </c>
       <c r="C5">
         <v>71233212332</v>
       </c>
@@ -527,6 +540,12 @@
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>21</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C7">
+        <v>81233214323</v>
       </c>
     </row>
   </sheetData>
@@ -542,6 +561,8 @@
     <hyperlink ref="E6" r:id="rId9" xr:uid="{BD6DD78D-D66B-458D-BCD7-E7B691C87772}"/>
     <hyperlink ref="E5" r:id="rId10" xr:uid="{DFA15038-6F28-4993-A104-5C9CEC9EC238}"/>
     <hyperlink ref="E4" r:id="rId11" xr:uid="{D4D42470-A725-40C4-9A4B-2B808DD433B4}"/>
+    <hyperlink ref="B5" r:id="rId12" xr:uid="{3D47A279-9C71-404D-864C-73028A4F9FAA}"/>
+    <hyperlink ref="B7" r:id="rId13" xr:uid="{C86C3DFC-749B-43CC-9F92-1500A2576615}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>